<commit_message>
Update excel test case
</commit_message>
<xml_diff>
--- a/doc/Test Cases.xlsx
+++ b/doc/Test Cases.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mario's PC\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2122-10-biology-KSChervenkov19\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5C54B55-B4E2-4047-B108-B2684AD4CB13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8DB0FCD-A633-4E07-A375-B782E97844FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="841" xr2:uid="{D96EB1AC-1A23-4874-8F12-F051FA81C7C1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>Test case 1</t>
   </si>
@@ -104,15 +104,9 @@
     <t>BLOCKED</t>
   </si>
   <si>
-    <t>Test Suite 1 - Automated testing of functions read/write data</t>
-  </si>
-  <si>
     <t>SS-001</t>
   </si>
   <si>
-    <t>getStatisticsFrom</t>
-  </si>
-  <si>
     <t>Testing the function which get statistics from a json file</t>
   </si>
   <si>
@@ -125,10 +119,19 @@
     <t>07/04/2021 07:52 PM</t>
   </si>
   <si>
-    <t>json_test_1.json</t>
-  </si>
-  <si>
     <t>It returns a proper array data from the .json file</t>
+  </si>
+  <si>
+    <t>Test.json</t>
+  </si>
+  <si>
+    <t>08/04/2021 02:41 PM</t>
+  </si>
+  <si>
+    <t>Test Suite 1 - Automated testing of functions read/write json data</t>
+  </si>
+  <si>
+    <t>getStatisticsFrom1</t>
   </si>
 </sst>
 </file>
@@ -497,7 +500,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
@@ -537,11 +540,23 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="22" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="24" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -549,17 +564,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="24" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -569,6 +575,9 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -589,9 +598,6 @@
           <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -615,7 +621,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E823A22D-AEBF-48ED-9EE6-4BAA3280E420}" name="Table1" displayName="Table1" ref="C10:I12" totalsRowShown="0">
   <autoFilter ref="C10:I12" xr:uid="{CBBAEA08-DC56-4B68-8DF5-9A2681C57DD3}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{F045B738-BC81-4AB6-A946-596415D46A39}" name="#" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{F045B738-BC81-4AB6-A946-596415D46A39}" name="#" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{E795166C-74FC-459A-AF28-E24B4C06703E}" name="Description"/>
     <tableColumn id="3" xr3:uid="{CD2CBAEA-36D3-4704-B133-871306A74BA7}" name="Test Data"/>
     <tableColumn id="4" xr3:uid="{19AD3074-2DAA-41E5-89A4-89C039D79A2C}" name="Expectations"/>
@@ -926,8 +932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E700B86-A081-4DFE-BEA1-995AE76D7104}">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -943,12 +949,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
+      <c r="A1" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
       <c r="E1" s="2"/>
       <c r="F1" s="3"/>
     </row>
@@ -965,12 +971,12 @@
         <v>0</v>
       </c>
       <c r="B3" s="4"/>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="27"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="27"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="30"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
@@ -979,13 +985,13 @@
         <v>2</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>3</v>
       </c>
       <c r="F4" s="21" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -995,42 +1001,42 @@
         <v>4</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>5</v>
       </c>
       <c r="F5" s="23" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G5" s="22"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="26"/>
-      <c r="C6" s="33" t="s">
+      <c r="C6" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="29" t="s">
-        <v>25</v>
+      <c r="D6" s="33" t="s">
+        <v>23</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>7</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="26"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="30"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="34"/>
       <c r="E7" s="12" t="s">
         <v>8</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1067,14 +1073,14 @@
       <c r="D11" t="s">
         <v>15</v>
       </c>
-      <c r="E11" t="s">
-        <v>29</v>
+      <c r="E11" s="35" t="s">
+        <v>28</v>
       </c>
       <c r="G11" t="s">
         <v>16</v>
       </c>
       <c r="H11" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1092,10 +1098,10 @@
         <v>16</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I12" s="18" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1115,13 +1121,13 @@
     <mergeCell ref="D6:D7"/>
   </mergeCells>
   <conditionalFormatting sqref="C11:I12 C15:I15">
-    <cfRule type="expression" dxfId="2" priority="13">
+    <cfRule type="expression" dxfId="3" priority="13">
       <formula>$H11="BLOCKED"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="14">
+    <cfRule type="expression" dxfId="2" priority="14">
       <formula>$H11="FAILED"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="15">
+    <cfRule type="expression" dxfId="1" priority="15">
       <formula>$H11="PASSED"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Create a test for the function which gets the .json file's names
</commit_message>
<xml_diff>
--- a/doc/Test Cases.xlsx
+++ b/doc/Test Cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2122-10-biology-KSChervenkov19\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8DB0FCD-A633-4E07-A375-B782E97844FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{879D41BE-3A16-4D51-99DC-F66D36C3A6D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="841" xr2:uid="{D96EB1AC-1A23-4874-8F12-F051FA81C7C1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="841" xr2:uid="{D96EB1AC-1A23-4874-8F12-F051FA81C7C1}"/>
   </bookViews>
   <sheets>
     <sheet name="SS-read-write-data-json" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="39">
   <si>
     <t>Test case 1</t>
   </si>
@@ -128,10 +128,31 @@
     <t>08/04/2021 02:41 PM</t>
   </si>
   <si>
-    <t>Test Suite 1 - Automated testing of functions read/write json data</t>
-  </si>
-  <si>
     <t>getStatisticsFrom1</t>
+  </si>
+  <si>
+    <t>Test Suite 1 - Automated testing of functions read/write json file data</t>
+  </si>
+  <si>
+    <t>SS-002</t>
+  </si>
+  <si>
+    <t>getStatisticsNames1</t>
+  </si>
+  <si>
+    <t>Testing the function which gets the file's names with extension .json</t>
+  </si>
+  <si>
+    <t>12/04/2021 05:53 PM</t>
+  </si>
+  <si>
+    <t>Test0.json, Test1.json, Test2.json, Test3.json</t>
+  </si>
+  <si>
+    <t>It returns a proper array of strings cointaining the names of the .json files which hold statistics data</t>
+  </si>
+  <si>
+    <t>Test case 2</t>
   </si>
 </sst>
 </file>
@@ -540,6 +561,9 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="22" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -564,9 +588,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20% - Accent1" xfId="3" builtinId="30"/>
@@ -574,7 +595,73 @@
     <cellStyle name="Heading 2" xfId="2" builtinId="17"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="14">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFA7A7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFA7A7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFA7A7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -621,13 +708,29 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E823A22D-AEBF-48ED-9EE6-4BAA3280E420}" name="Table1" displayName="Table1" ref="C10:I12" totalsRowShown="0">
   <autoFilter ref="C10:I12" xr:uid="{CBBAEA08-DC56-4B68-8DF5-9A2681C57DD3}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{F045B738-BC81-4AB6-A946-596415D46A39}" name="#" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{F045B738-BC81-4AB6-A946-596415D46A39}" name="#" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{E795166C-74FC-459A-AF28-E24B4C06703E}" name="Description"/>
     <tableColumn id="3" xr3:uid="{CD2CBAEA-36D3-4704-B133-871306A74BA7}" name="Test Data"/>
     <tableColumn id="4" xr3:uid="{19AD3074-2DAA-41E5-89A4-89C039D79A2C}" name="Expectations"/>
     <tableColumn id="5" xr3:uid="{D363DF36-08AD-4B92-A469-91367ED37232}" name="Actual Result"/>
     <tableColumn id="6" xr3:uid="{080E491F-2510-42BF-8E17-4241A5BDDF57}" name="Status"/>
     <tableColumn id="7" xr3:uid="{8E8AB07E-B2AE-4D4A-ACE0-537C62C88924}" name="Comments"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A0630AD4-6082-455E-AA23-092ABE4DD88D}" name="Table15" displayName="Table15" ref="C24:I26" totalsRowShown="0">
+  <autoFilter ref="C24:I26" xr:uid="{A0630AD4-6082-455E-AA23-092ABE4DD88D}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{29161239-8648-433E-8E7F-327F36E7512F}" name="#" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{BB3C46E8-1FE6-4CF7-96C1-9567CE973A58}" name="Description"/>
+    <tableColumn id="3" xr3:uid="{A4D3DB36-599D-4BE5-ABAA-81C0E54D63AD}" name="Test Data"/>
+    <tableColumn id="4" xr3:uid="{2C8185FA-9CE4-4187-A130-5B1F09C6E6C0}" name="Expectations"/>
+    <tableColumn id="5" xr3:uid="{AC6A0C8E-A9F5-4D9D-AA13-5F6CC6B0DC78}" name="Actual Result"/>
+    <tableColumn id="6" xr3:uid="{EFA33CBC-967C-44D7-8BEB-BE684E83353D}" name="Status"/>
+    <tableColumn id="7" xr3:uid="{A2BA86E3-F405-4E3C-8227-854AD8392864}" name="Comments"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -930,35 +1033,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E700B86-A081-4DFE-BEA1-995AE76D7104}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="64.7109375" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1"/>
-    <col min="6" max="6" width="56.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="33.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="64.6640625" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" customWidth="1"/>
+    <col min="6" max="6" width="56.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
+    <row r="1" spans="1:9" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="A1" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
       <c r="E1" s="2"/>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="5"/>
@@ -966,19 +1069,19 @@
       <c r="E2" s="4"/>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="4"/>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="30"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="30"/>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D3" s="31"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="31"/>
+    </row>
+    <row r="4" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="24" t="s">
@@ -994,14 +1097,14 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="26"/>
       <c r="C5" s="25" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>5</v>
@@ -1011,13 +1114,13 @@
       </c>
       <c r="G5" s="22"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="26"/>
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="33" t="s">
+      <c r="D6" s="34" t="s">
         <v>23</v>
       </c>
       <c r="E6" s="11" t="s">
@@ -1027,11 +1130,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="26"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="34"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="35"/>
       <c r="E7" s="12" t="s">
         <v>8</v>
       </c>
@@ -1039,11 +1142,11 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D8" s="20"/>
       <c r="F8" s="20"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C10" s="13" t="s">
         <v>9</v>
       </c>
@@ -1066,14 +1169,14 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C11" s="14">
         <v>1</v>
       </c>
       <c r="D11" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="35" t="s">
+      <c r="E11" s="27" t="s">
         <v>28</v>
       </c>
       <c r="G11" t="s">
@@ -1083,7 +1186,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C12" s="15">
         <v>2</v>
       </c>
@@ -1104,7 +1207,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C15" s="15"/>
       <c r="D15" s="16"/>
       <c r="E15" s="17"/>
@@ -1113,27 +1216,180 @@
       <c r="H15" s="16"/>
       <c r="I15" s="18"/>
     </row>
+    <row r="17" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="31"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="31"/>
+    </row>
+    <row r="18" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18" s="21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="4"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="G19" s="22"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="4"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="4"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D22" s="20"/>
+      <c r="F22" s="20"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C24" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" t="s">
+        <v>12</v>
+      </c>
+      <c r="H24" t="s">
+        <v>13</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C25" s="14">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="G25" t="s">
+        <v>16</v>
+      </c>
+      <c r="H25" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C26" s="15">
+        <v>2</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E26" s="17"/>
+      <c r="F26" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="G26" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H26" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="I26" s="18" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="7">
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="C3:F3"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:D7"/>
   </mergeCells>
   <conditionalFormatting sqref="C11:I12 C15:I15">
-    <cfRule type="expression" dxfId="3" priority="13">
+    <cfRule type="expression" dxfId="13" priority="16">
       <formula>$H11="BLOCKED"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="14">
+    <cfRule type="expression" dxfId="12" priority="17">
       <formula>$H11="FAILED"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="15">
+    <cfRule type="expression" dxfId="11" priority="18">
       <formula>$H11="PASSED"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C25:I26">
+    <cfRule type="expression" dxfId="3" priority="1">
+      <formula>$H25="BLOCKED"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>$H25="FAILED"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="3">
+      <formula>$H25="PASSED"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -1142,7 +1398,7 @@
           <x14:formula1>
             <xm:f>'Values for status dropdown'!$A$1:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>H11:H12 H15</xm:sqref>
+          <xm:sqref>H11:H12 H15 H25:H26</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1158,19 +1414,19 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
Add tests for the bll getter .json data functions
</commit_message>
<xml_diff>
--- a/doc/Test Cases.xlsx
+++ b/doc/Test Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2122-10-biology-KSChervenkov19\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{879D41BE-3A16-4D51-99DC-F66D36C3A6D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{276C21A4-B36D-4B77-A449-C326D9C399F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="841" xr2:uid="{D96EB1AC-1A23-4874-8F12-F051FA81C7C1}"/>
   </bookViews>
@@ -122,24 +122,15 @@
     <t>It returns a proper array data from the .json file</t>
   </si>
   <si>
-    <t>Test.json</t>
-  </si>
-  <si>
     <t>08/04/2021 02:41 PM</t>
   </si>
   <si>
-    <t>getStatisticsFrom1</t>
-  </si>
-  <si>
     <t>Test Suite 1 - Automated testing of functions read/write json file data</t>
   </si>
   <si>
     <t>SS-002</t>
   </si>
   <si>
-    <t>getStatisticsNames1</t>
-  </si>
-  <si>
     <t>Testing the function which gets the file's names with extension .json</t>
   </si>
   <si>
@@ -153,6 +144,15 @@
   </si>
   <si>
     <t>Test case 2</t>
+  </si>
+  <si>
+    <t>Test0.json</t>
+  </si>
+  <si>
+    <t>getStatisticsNames1 / getStatisticsNames2</t>
+  </si>
+  <si>
+    <t>getStatisticsFrom1 / getStatisticsFrom1</t>
   </si>
 </sst>
 </file>
@@ -1036,7 +1036,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1053,7 +1053,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A1" s="28" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B1" s="29"/>
       <c r="C1" s="29"/>
@@ -1104,7 +1104,7 @@
         <v>4</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>5</v>
@@ -1139,7 +1139,7 @@
         <v>8</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -1177,7 +1177,7 @@
         <v>15</v>
       </c>
       <c r="E11" s="27" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="G11" t="s">
         <v>16</v>
@@ -1218,7 +1218,7 @@
     </row>
     <row r="17" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="30" t="s">
@@ -1235,7 +1235,7 @@
         <v>2</v>
       </c>
       <c r="D18" s="21" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>3</v>
@@ -1251,13 +1251,13 @@
         <v>4</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>5</v>
       </c>
       <c r="F19" s="23" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G19" s="22"/>
     </row>
@@ -1268,7 +1268,7 @@
         <v>6</v>
       </c>
       <c r="D20" s="34" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E20" s="11" t="s">
         <v>7</v>
@@ -1286,7 +1286,7 @@
         <v>8</v>
       </c>
       <c r="F21" s="19" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
@@ -1324,7 +1324,7 @@
         <v>15</v>
       </c>
       <c r="E25" s="27" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G25" t="s">
         <v>16</v>
@@ -1351,7 +1351,7 @@
         <v>17</v>
       </c>
       <c r="I26" s="18" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>